<commit_message>
Updated readme with how to use.
</commit_message>
<xml_diff>
--- a/documentation/gv_pipeline_documentation.xlsx
+++ b/documentation/gv_pipeline_documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarpy\Documents\portfolio_projects\gv_break_risk_pipeline\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B57AE4-BCEA-4199-B43F-06B82BA72A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C28CD7-CAB7-4A10-AEAC-477F5A9CA42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{EAAC5EBF-1D59-4464-823D-D4AD62A2C644}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EAAC5EBF-1D59-4464-823D-D4AD62A2C644}"/>
   </bookViews>
   <sheets>
     <sheet name="data_info" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>Unique identifier for each employee (eg E001, E002,…)</t>
   </si>
   <si>
-    <t>Work date for the timecard entry (YYY-MM-DD)</t>
-  </si>
-  <si>
     <t>Timestamp when the employee started their shift</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>7 rows removed until corrected</t>
+  </si>
+  <si>
+    <t>Work date for the timecard entry (YYYY-MM-DD)</t>
   </si>
 </sst>
 </file>
@@ -140,9 +140,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]mmmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\-yy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,16 +150,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -167,11 +180,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -182,20 +210,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -203,16 +237,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -556,106 +580,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772B93A2-F892-4551-BE1A-E9FE23E5B03F}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="B2:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.44140625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="26.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="44.44140625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="2:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D3" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D4" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="D8" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1" t="s">
+    <row r="9" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -667,7 +692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86983184-989D-4277-B3D8-61B023A27F89}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:G2"/>
     </sheetView>
   </sheetViews>
@@ -685,28 +710,28 @@
   <sheetData>
     <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -717,7 +742,7 @@
         <v>400</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2">
         <v>7</v>
@@ -732,12 +757,12 @@
         <v>161</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>